<commit_message>
Update the resources to follow the recent changes in the lecture
</commit_message>
<xml_diff>
--- a/cellfie/Working-Samples/grocery-item.xlsx
+++ b/cellfie/Working-Samples/grocery-item.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="491"/>
+    <workbookView xWindow="9120" yWindow="3020" windowWidth="24500" windowHeight="12960" tabRatio="378" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Grocery Items" sheetId="1" r:id="rId1"/>
     <sheet name="Food Ingredient" sheetId="2" r:id="rId2"/>
     <sheet name="Nutritional Info" sheetId="3" r:id="rId3"/>
+    <sheet name="Food Stuff Organization" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="187">
   <si>
     <t>Grocery Item</t>
   </si>
@@ -62,7 +63,7 @@
     <t>Lotus Biscoff Cookies Item</t>
   </si>
   <si>
-    <t>Lotus Biscoff Cookies</t>
+    <t>Biscoff Cookie</t>
   </si>
   <si>
     <t>For decades, Lotus Biscoff Cookies has been Europe's favorite cookie to enjoy with coffee. Their popularity in the U.S. spread when this crisp, delicious cookie began to be served on airplanes.</t>
@@ -107,18 +108,6 @@
     <t>http://i.imgur.com/CRWoRjT.jpg</t>
   </si>
   <si>
-    <t>Heinz Beans with Tomato Sauce Item</t>
-  </si>
-  <si>
-    <t>Heinz Beans with Tomato Sauce</t>
-  </si>
-  <si>
-    <t>Heinz Beans with Tomato Sauce are premium vegetarian beans in a rich flavorful sauce that can be eaten as a side dish or by themselves. The beans with sauce are offered in a 13.7-oz can (pack of 12) for your convenience. Heinz beans are an excellent source of fiber, suitable for vegetarians and contain no artificial colors, preservatives or flavors. These Heinz Beans with Tomato Sauce contain no cholesterol.</t>
-  </si>
-  <si>
-    <t>http://i.imgur.com/IbNS6JL.jpg</t>
-  </si>
-  <si>
     <t>Kashi Crunch Chocolate Chip Bar Item</t>
   </si>
   <si>
@@ -371,18 +360,6 @@
     <t>Zinc</t>
   </si>
   <si>
-    <t>Bean</t>
-  </si>
-  <si>
-    <t>Onion</t>
-  </si>
-  <si>
-    <t>Spice</t>
-  </si>
-  <si>
-    <t>Tomato</t>
-  </si>
-  <si>
     <t>Barley</t>
   </si>
   <si>
@@ -572,9 +549,6 @@
     <t>0 mg</t>
   </si>
   <si>
-    <t>440 mg</t>
-  </si>
-  <si>
     <t>100 mg</t>
   </si>
   <si>
@@ -591,13 +565,31 @@
   </si>
   <si>
     <t>50 mg</t>
+  </si>
+  <si>
+    <t>FoodStuff</t>
+  </si>
+  <si>
+    <t>(Super-)Category</t>
+  </si>
+  <si>
+    <t>Cookie</t>
+  </si>
+  <si>
+    <t>Cereal</t>
+  </si>
+  <si>
+    <t>Cereal Bar</t>
+  </si>
+  <si>
+    <t>Shortbread</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -630,6 +622,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
@@ -668,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -681,6 +678,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1021,18 +1022,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="64.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.6640625" customWidth="1"/>
-    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="23">
@@ -1147,14 +1145,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18">
+    <row r="9" spans="1:4" ht="18">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1168,7 +1166,7 @@
       <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1185,7 +1183,7 @@
       <c r="C11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1199,7 +1197,7 @@
       <c r="C12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1215,20 +1213,6 @@
       </c>
       <c r="D13" s="4" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="18">
-      <c r="A14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1244,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK165"/>
+  <dimension ref="A1:AMK158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B160" sqref="B160"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:XFD79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1262,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1270,7 +1254,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1278,7 +1262,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1286,7 +1270,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1294,7 +1278,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1302,7 +1286,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1310,7 +1294,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1318,7 +1302,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1326,7 +1310,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1334,7 +1318,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1342,7 +1326,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1350,7 +1334,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1358,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1366,7 +1350,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1374,7 +1358,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1382,7 +1366,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1390,7 +1374,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1398,71 +1382,71 @@
         <v>9</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="B26" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1470,7 +1454,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1478,7 +1462,7 @@
         <v>17</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1486,7 +1470,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1494,7 +1478,7 @@
         <v>17</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1502,7 +1486,7 @@
         <v>17</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1510,55 +1494,55 @@
         <v>17</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1566,7 +1550,7 @@
         <v>21</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1574,7 +1558,7 @@
         <v>21</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1582,7 +1566,7 @@
         <v>21</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1590,7 +1574,7 @@
         <v>21</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1598,7 +1582,7 @@
         <v>21</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1606,7 +1590,7 @@
         <v>21</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1614,7 +1598,7 @@
         <v>21</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1622,7 +1606,7 @@
         <v>21</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1630,7 +1614,7 @@
         <v>21</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1638,7 +1622,7 @@
         <v>21</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1646,39 +1630,39 @@
         <v>21</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1686,7 +1670,7 @@
         <v>25</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1694,7 +1678,7 @@
         <v>25</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1702,7 +1686,7 @@
         <v>25</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1710,7 +1694,7 @@
         <v>25</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1718,7 +1702,7 @@
         <v>25</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1726,7 +1710,7 @@
         <v>25</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1734,7 +1718,7 @@
         <v>25</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1742,7 +1726,7 @@
         <v>25</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1750,7 +1734,7 @@
         <v>25</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1758,7 +1742,7 @@
         <v>25</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1766,7 +1750,7 @@
         <v>25</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1774,7 +1758,7 @@
         <v>25</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1782,7 +1766,7 @@
         <v>25</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1790,7 +1774,7 @@
         <v>25</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1798,7 +1782,7 @@
         <v>25</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1806,7 +1790,7 @@
         <v>25</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1814,7 +1798,7 @@
         <v>25</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1822,7 +1806,7 @@
         <v>25</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1830,247 +1814,247 @@
         <v>25</v>
       </c>
       <c r="B72" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="3" t="s">
+    <row r="78" spans="1:2">
+      <c r="A78" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B78" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="3" t="s">
+    <row r="79" spans="1:2">
+      <c r="A79" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B74" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B75" s="6" t="s">
+      <c r="B79" s="6" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B92" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="6" t="s">
+      <c r="B93" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="6" t="s">
+      <c r="B94" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B94" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="6" t="s">
+      <c r="B95" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="6" t="s">
+      <c r="B96" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B96" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="6" t="s">
+      <c r="B97" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B97" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="6" t="s">
+      <c r="B98" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B98" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="B99" s="6" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2078,7 +2062,7 @@
         <v>37</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2086,7 +2070,7 @@
         <v>37</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2094,7 +2078,7 @@
         <v>37</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2102,7 +2086,7 @@
         <v>37</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2110,7 +2094,7 @@
         <v>37</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2118,7 +2102,7 @@
         <v>37</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2126,327 +2110,327 @@
         <v>37</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B112" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="3" t="s">
+      <c r="B113" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B113" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="3" t="s">
+      <c r="B114" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B114" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="3" t="s">
+      <c r="B115" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B115" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="3" t="s">
+      <c r="B116" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B116" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="3" t="s">
+      <c r="B117" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B117" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="3" t="s">
+      <c r="B118" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B118" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="B119" s="6" t="s">
-        <v>64</v>
+        <v>141</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>147</v>
+        <v>68</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="6" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="6" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="6" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="6" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>151</v>
+        <v>60</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="6" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="6" t="s">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>152</v>
+        <v>96</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="6" t="s">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="6" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="6" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>154</v>
+        <v>57</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="6" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="6" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>64</v>
+        <v>139</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="6" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>157</v>
+        <v>92</v>
       </c>
     </row>
     <row r="140" spans="1:2">
-      <c r="A140" s="6" t="s">
-        <v>141</v>
+      <c r="A140" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="141" spans="1:2">
-      <c r="A141" s="6" t="s">
-        <v>141</v>
+      <c r="A141" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
     </row>
     <row r="142" spans="1:2">
-      <c r="A142" s="6" t="s">
-        <v>153</v>
+      <c r="A142" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
     </row>
     <row r="143" spans="1:2">
-      <c r="A143" s="6" t="s">
-        <v>153</v>
+      <c r="A143" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>147</v>
+        <v>71</v>
       </c>
     </row>
     <row r="144" spans="1:2">
-      <c r="A144" s="6" t="s">
-        <v>153</v>
+      <c r="A144" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
     </row>
     <row r="145" spans="1:2">
-      <c r="A145" s="6" t="s">
-        <v>153</v>
+      <c r="A145" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="146" spans="1:2">
-      <c r="A146" s="6" t="s">
-        <v>153</v>
+      <c r="A146" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2454,7 +2438,7 @@
         <v>49</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>75</v>
+        <v>140</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2462,7 +2446,7 @@
         <v>49</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2470,7 +2454,7 @@
         <v>49</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2478,103 +2462,47 @@
         <v>49</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="154" spans="1:2">
-      <c r="A154" s="3" t="s">
-        <v>49</v>
+      <c r="A154" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>163</v>
+        <v>96</v>
       </c>
     </row>
     <row r="155" spans="1:2">
-      <c r="A155" s="3" t="s">
-        <v>49</v>
+      <c r="A155" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="156" spans="1:2">
-      <c r="A156" s="3" t="s">
-        <v>49</v>
+      <c r="A156" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>72</v>
+        <v>157</v>
       </c>
     </row>
     <row r="157" spans="1:2">
-      <c r="A157" s="3" t="s">
-        <v>53</v>
+      <c r="A157" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>148</v>
+        <v>60</v>
       </c>
     </row>
     <row r="158" spans="1:2">
-      <c r="A158" s="3" t="s">
-        <v>53</v>
+      <c r="A158" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2">
-      <c r="A159" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B159" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2">
-      <c r="A160" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B160" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2">
-      <c r="A161" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B161" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2">
-      <c r="A162" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B162" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2">
-      <c r="A163" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B163" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2">
-      <c r="A164" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B164" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2">
-      <c r="A165" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B165" s="6" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2590,113 +2518,103 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK14"/>
+  <dimension ref="A1:AMK13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="7"/>
-    <col min="4" max="4" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="7" customWidth="1"/>
-    <col min="11" max="12" width="14.1640625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" style="7" customWidth="1"/>
-    <col min="14" max="1025" width="8.83203125" style="7"/>
+    <col min="1" max="1" width="35.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="1025" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="52" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:14" s="10" customFormat="1" ht="52" customHeight="1">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="K1" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="L1" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="M1" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="N1" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="6" customFormat="1" ht="18">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="12">
         <v>7</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="12">
         <v>4.5</v>
       </c>
-      <c r="D2" s="10">
-        <v>0</v>
-      </c>
-      <c r="E2" s="10">
-        <v>0</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="G2" s="10">
+      <c r="D2" s="12">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" s="12">
         <v>21</v>
       </c>
-      <c r="H2" s="10">
-        <v>0</v>
-      </c>
-      <c r="I2" s="10">
+      <c r="H2" s="12">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12">
         <v>12</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="12">
         <v>1</v>
       </c>
-      <c r="K2" s="10">
-        <v>0</v>
-      </c>
-      <c r="L2" s="10">
-        <v>0</v>
-      </c>
-      <c r="M2" s="10">
-        <v>0</v>
-      </c>
-      <c r="N2" s="10">
+      <c r="K2" s="12">
+        <v>0</v>
+      </c>
+      <c r="L2" s="12">
+        <v>0</v>
+      </c>
+      <c r="M2" s="12">
+        <v>0</v>
+      </c>
+      <c r="N2" s="12">
         <v>6</v>
       </c>
     </row>
@@ -2704,87 +2622,87 @@
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="12">
         <v>1</v>
       </c>
-      <c r="C3" s="10">
-        <v>0</v>
-      </c>
-      <c r="D3" s="10">
-        <v>0</v>
-      </c>
-      <c r="E3" s="10">
-        <v>0</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="G3" s="10">
+      <c r="C3" s="12">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="12">
         <v>25</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="12">
         <v>3</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="12">
         <v>6</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="12">
         <v>2</v>
       </c>
-      <c r="K3" s="10">
-        <v>0</v>
-      </c>
-      <c r="L3" s="10">
-        <v>0</v>
-      </c>
-      <c r="M3" s="10">
+      <c r="K3" s="12">
+        <v>0</v>
+      </c>
+      <c r="L3" s="12">
+        <v>0</v>
+      </c>
+      <c r="M3" s="12">
         <v>10</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="6" customFormat="1" ht="18">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="12">
         <v>6</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="12">
         <v>3</v>
       </c>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="G4" s="10">
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G4" s="12">
         <v>23</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="12">
         <v>0.4</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="12">
         <v>12</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="12">
         <v>2</v>
       </c>
-      <c r="K4" s="10">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10">
-        <v>0</v>
-      </c>
-      <c r="M4" s="10">
+      <c r="K4" s="12">
+        <v>0</v>
+      </c>
+      <c r="L4" s="12">
+        <v>0</v>
+      </c>
+      <c r="M4" s="12">
         <v>1</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="12">
         <v>1</v>
       </c>
     </row>
@@ -2792,43 +2710,43 @@
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="12">
         <v>4</v>
       </c>
-      <c r="C5" s="10">
-        <v>0</v>
-      </c>
-      <c r="D5" s="10">
-        <v>0</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G5" s="12">
         <v>41</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="12">
         <v>5</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="12">
         <v>3</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="12">
         <v>7</v>
       </c>
-      <c r="K5" s="10">
-        <v>0</v>
-      </c>
-      <c r="L5" s="10">
-        <v>0</v>
-      </c>
-      <c r="M5" s="10">
+      <c r="K5" s="12">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0</v>
+      </c>
+      <c r="M5" s="12">
         <v>4</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="12">
         <v>15</v>
       </c>
     </row>
@@ -2836,43 +2754,43 @@
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="12">
         <v>3</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="12">
         <v>0.5</v>
       </c>
-      <c r="D6" s="10">
-        <v>0</v>
-      </c>
-      <c r="E6" s="10">
-        <v>0</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="G6" s="10">
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="G6" s="12">
         <v>41</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="12">
         <v>4</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="12">
         <v>7</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="12">
         <v>6</v>
       </c>
-      <c r="K6" s="10">
-        <v>0</v>
-      </c>
-      <c r="L6" s="10">
-        <v>0</v>
-      </c>
-      <c r="M6" s="10">
+      <c r="K6" s="12">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12">
         <v>2</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="12">
         <v>15</v>
       </c>
     </row>
@@ -2880,43 +2798,43 @@
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="12">
         <v>2</v>
       </c>
-      <c r="C7" s="10">
-        <v>0</v>
-      </c>
-      <c r="D7" s="10">
-        <v>0</v>
-      </c>
-      <c r="E7" s="10">
-        <v>0</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="G7" s="10">
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="G7" s="12">
         <v>20</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="12">
         <v>3</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="12">
         <v>1</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="12">
         <v>3</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="12">
         <v>10</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="12">
         <v>10</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="12">
         <v>10</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="12">
         <v>45</v>
       </c>
     </row>
@@ -2924,307 +2842,263 @@
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="10">
-        <v>0</v>
-      </c>
-      <c r="C8" s="10">
-        <v>0</v>
-      </c>
-      <c r="D8" s="10">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10">
-        <v>0</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="G8" s="10">
-        <v>18</v>
-      </c>
-      <c r="H8" s="10">
-        <v>5</v>
-      </c>
-      <c r="I8" s="10">
+      <c r="B8" s="12">
         <v>7</v>
       </c>
-      <c r="J8" s="10">
+      <c r="C8" s="12">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="12">
+        <v>27</v>
+      </c>
+      <c r="H8" s="12">
+        <v>3</v>
+      </c>
+      <c r="I8" s="12">
+        <v>9</v>
+      </c>
+      <c r="J8" s="12">
+        <v>3</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0</v>
+      </c>
+      <c r="M8" s="12">
+        <v>2</v>
+      </c>
+      <c r="N8" s="12">
         <v>6</v>
-      </c>
-      <c r="K8" s="10">
-        <v>0</v>
-      </c>
-      <c r="L8" s="10">
-        <v>0</v>
-      </c>
-      <c r="M8" s="10">
-        <v>6</v>
-      </c>
-      <c r="N8" s="10">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="6" customFormat="1" ht="18">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="10">
-        <v>7</v>
-      </c>
-      <c r="C9" s="10">
+      <c r="B9" s="12">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" s="12">
+        <v>29</v>
+      </c>
+      <c r="H9" s="12">
+        <v>1</v>
+      </c>
+      <c r="I9" s="12">
+        <v>4</v>
+      </c>
+      <c r="J9" s="12">
         <v>2</v>
       </c>
-      <c r="D9" s="10">
-        <v>0</v>
-      </c>
-      <c r="E9" s="10">
-        <v>0</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="G9" s="10">
-        <v>27</v>
-      </c>
-      <c r="H9" s="10">
-        <v>3</v>
-      </c>
-      <c r="I9" s="10">
-        <v>9</v>
-      </c>
-      <c r="J9" s="10">
-        <v>3</v>
-      </c>
-      <c r="K9" s="10">
-        <v>0</v>
-      </c>
-      <c r="L9" s="10">
-        <v>0</v>
-      </c>
-      <c r="M9" s="10">
-        <v>2</v>
-      </c>
-      <c r="N9" s="10">
-        <v>6</v>
+      <c r="K9" s="12">
+        <v>25</v>
+      </c>
+      <c r="L9" s="12">
+        <v>25</v>
+      </c>
+      <c r="M9" s="12">
+        <v>0</v>
+      </c>
+      <c r="N9" s="12">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="6" customFormat="1" ht="18">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="10">
-        <v>0</v>
-      </c>
-      <c r="D10" s="10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="G10" s="10">
-        <v>29</v>
-      </c>
-      <c r="H10" s="10">
+      <c r="B10" s="12">
+        <v>9</v>
+      </c>
+      <c r="C10" s="12">
+        <v>3</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="12">
+        <v>18</v>
+      </c>
+      <c r="H10" s="12">
         <v>1</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="12">
+        <v>12</v>
+      </c>
+      <c r="J10" s="12">
+        <v>1</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <v>0</v>
+      </c>
+      <c r="N10" s="12">
         <v>4</v>
-      </c>
-      <c r="J10" s="10">
-        <v>2</v>
-      </c>
-      <c r="K10" s="10">
-        <v>25</v>
-      </c>
-      <c r="L10" s="10">
-        <v>25</v>
-      </c>
-      <c r="M10" s="10">
-        <v>0</v>
-      </c>
-      <c r="N10" s="10">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="6" customFormat="1" ht="18">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="10">
-        <v>9</v>
-      </c>
-      <c r="C11" s="10">
-        <v>3</v>
-      </c>
-      <c r="D11" s="10">
-        <v>0</v>
-      </c>
-      <c r="E11" s="10">
-        <v>0</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="G11" s="10">
-        <v>18</v>
-      </c>
-      <c r="H11" s="10">
+      <c r="B11" s="12">
+        <v>6</v>
+      </c>
+      <c r="C11" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0</v>
+      </c>
+      <c r="E11" s="12">
+        <v>5</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G11" s="12">
+        <v>17</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12">
+        <v>10</v>
+      </c>
+      <c r="J11" s="12">
         <v>1</v>
       </c>
-      <c r="I11" s="10">
-        <v>12</v>
-      </c>
-      <c r="J11" s="10">
-        <v>1</v>
-      </c>
-      <c r="K11" s="10">
-        <v>0</v>
-      </c>
-      <c r="L11" s="10">
-        <v>0</v>
-      </c>
-      <c r="M11" s="10">
-        <v>0</v>
-      </c>
-      <c r="N11" s="10">
-        <v>4</v>
+      <c r="K11" s="12">
+        <v>0</v>
+      </c>
+      <c r="L11" s="12">
+        <v>0</v>
+      </c>
+      <c r="M11" s="12">
+        <v>0</v>
+      </c>
+      <c r="N11" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="6" customFormat="1" ht="18">
       <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="G12" s="12">
+        <v>26</v>
+      </c>
+      <c r="H12" s="12">
+        <v>5</v>
+      </c>
+      <c r="I12" s="12">
+        <v>9</v>
+      </c>
+      <c r="J12" s="12">
+        <v>2</v>
+      </c>
+      <c r="K12" s="12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <v>8</v>
+      </c>
+      <c r="N12" s="12">
         <v>6</v>
-      </c>
-      <c r="C12" s="10">
-        <v>3.5</v>
-      </c>
-      <c r="D12" s="10">
-        <v>0</v>
-      </c>
-      <c r="E12" s="10">
-        <v>5</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="G12" s="10">
-        <v>17</v>
-      </c>
-      <c r="H12" s="10">
-        <v>0</v>
-      </c>
-      <c r="I12" s="10">
-        <v>10</v>
-      </c>
-      <c r="J12" s="10">
-        <v>1</v>
-      </c>
-      <c r="K12" s="10">
-        <v>0</v>
-      </c>
-      <c r="L12" s="10">
-        <v>0</v>
-      </c>
-      <c r="M12" s="10">
-        <v>0</v>
-      </c>
-      <c r="N12" s="10">
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="6" customFormat="1" ht="18">
       <c r="A13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="12">
+        <v>6</v>
+      </c>
+      <c r="C13" s="12">
+        <v>4</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12">
+        <v>15</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G13" s="12">
+        <v>11</v>
+      </c>
+      <c r="H13" s="12">
         <v>1</v>
       </c>
-      <c r="C13" s="10">
-        <v>0</v>
-      </c>
-      <c r="D13" s="10">
-        <v>0</v>
-      </c>
-      <c r="E13" s="10">
-        <v>0</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="G13" s="10">
-        <v>26</v>
-      </c>
-      <c r="H13" s="10">
-        <v>5</v>
-      </c>
-      <c r="I13" s="10">
-        <v>9</v>
-      </c>
-      <c r="J13" s="10">
-        <v>2</v>
-      </c>
-      <c r="K13" s="10">
-        <v>0</v>
-      </c>
-      <c r="L13" s="10">
-        <v>0</v>
-      </c>
-      <c r="M13" s="10">
-        <v>8</v>
-      </c>
-      <c r="N13" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="6" customFormat="1" ht="18">
-      <c r="A14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="10">
-        <v>6</v>
-      </c>
-      <c r="C14" s="10">
+      <c r="I13" s="12">
+        <v>3</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1</v>
+      </c>
+      <c r="K13" s="12">
         <v>4</v>
       </c>
-      <c r="D14" s="10">
-        <v>0</v>
-      </c>
-      <c r="E14" s="10">
-        <v>15</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="G14" s="10">
-        <v>11</v>
-      </c>
-      <c r="H14" s="10">
-        <v>1</v>
-      </c>
-      <c r="I14" s="10">
-        <v>3</v>
-      </c>
-      <c r="J14" s="10">
-        <v>1</v>
-      </c>
-      <c r="K14" s="10">
-        <v>4</v>
-      </c>
-      <c r="L14" s="10">
-        <v>0</v>
-      </c>
-      <c r="M14" s="10">
-        <v>0</v>
-      </c>
-      <c r="N14" s="10">
+      <c r="L13" s="12">
+        <v>0</v>
+      </c>
+      <c r="M13" s="12">
+        <v>0</v>
+      </c>
+      <c r="N13" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3237,4 +3111,138 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="23">
+      <c r="A1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" ht="18">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18">
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18">
+      <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18">
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18">
+      <c r="A9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18">
+      <c r="A10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18">
+      <c r="A11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18">
+      <c r="A12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18">
+      <c r="A13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>